<commit_message>
Drop ; in emails
</commit_message>
<xml_diff>
--- a/Список для обзвона/mass_fin.xlsx
+++ b/Список для обзвона/mass_fin.xlsx
@@ -3312,7 +3312,7 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t xml:space="preserve">urist@bryankonfi.ru; urist1@bryankonfi.ru </t>
+          <t xml:space="preserve">urist@bryankonfi.ru urist1@bryankonfi.ru </t>
         </is>
       </c>
     </row>
@@ -5716,7 +5716,7 @@
       </c>
       <c r="E238" t="inlineStr">
         <is>
-          <t>2207;vkim@marr.ru</t>
+          <t>vkim@marr.ru</t>
         </is>
       </c>
     </row>

</xml_diff>